<commit_message>
Debug - No Shallow Retrofit Limit
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_RSD_Retrofit-Ctrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B249EDCE-9072-4DE9-9C9A-F81909EEF1AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F03F403-3587-49C0-9BEF-B5C4560BFA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -752,15 +752,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -784,6 +775,15 @@
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1941,7 +1941,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:H23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2055,10 +2055,22 @@
         <f>"R-RTFT-"&amp;J9&amp;"_Shallow"</f>
         <v>R-RTFT-Apt_Shallow</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="D9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14">
+        <f>N21*F$15</f>
+        <v>0</v>
+      </c>
       <c r="G9" s="14">
         <f>(H22*G$15)/1000</f>
         <v>46.6311040684012</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>7</v>
@@ -2103,35 +2115,47 @@
         <f>"R-RTFT-"&amp;J11&amp;"_Shallow"</f>
         <v>R-RTFT-Att_Shallow</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="D11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14">
+        <f>N23*F$15</f>
+        <v>0</v>
+      </c>
       <c r="G11" s="14">
         <f>(F22*G$15)/1000</f>
         <v>223.3610244531846</v>
       </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
       <c r="J11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="str">
+      <c r="A12" s="31" t="str">
         <f>"UC_RSD_RetrofitCap-"&amp;J12</f>
         <v>UC_RSD_RetrofitCap-Det</v>
       </c>
-      <c r="B12" s="34" t="str">
+      <c r="B12" s="31" t="str">
         <f>"Maximum number of retrofitted dwellings in RSD "&amp;J12</f>
         <v>Maximum number of retrofitted dwellings in RSD Det</v>
       </c>
-      <c r="C12" s="34" t="str">
+      <c r="C12" s="31" t="str">
         <f>"R-RTFT-"&amp;J12&amp;"_Deep"</f>
         <v>R-RTFT-Det_Deep</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="31">
         <v>1</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="32">
         <f>N22*F$15</f>
         <v>0</v>
       </c>
@@ -2139,31 +2163,40 @@
         <f>(G23*G$15)/1000</f>
         <v>292.69993918242557</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="2">
         <v>5</v>
       </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34" t="s">
+      <c r="I12" s="31"/>
+      <c r="J12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36" t="str">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33" t="str">
         <f>"R-RTFT-"&amp;J13&amp;"_Shallow"</f>
         <v>R-RTFT-Det_Shallow</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37">
+      <c r="D13" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="33">
+        <v>1</v>
+      </c>
+      <c r="F13" s="34">
+        <f>N25*F$15</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="34">
         <f>(G22*G$15)/1000</f>
         <v>198.9528640113158</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34" t="s">
+      <c r="H13" s="33">
+        <v>5</v>
+      </c>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2182,16 +2215,16 @@
     <row r="18" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19"/>
-      <c r="C19" s="23">
+      <c r="C19" s="35">
         <v>2018</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="23">
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="35">
         <v>2070</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -2204,22 +2237,22 @@
     </row>
     <row r="20" spans="2:15" ht="15" x14ac:dyDescent="0.2">
       <c r="B20"/>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="23" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="23" t="s">
         <v>77</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="24" t="s">
         <v>79</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -2248,15 +2281,15 @@
       <c r="E21" s="22">
         <v>50844.518002144141</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="25">
         <f>C21*0.8333</f>
         <v>76933.418177245752</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="26">
         <f t="shared" ref="G21:H23" si="0">D21*0.8333</f>
         <v>86138.026655972135</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="27">
         <f t="shared" si="0"/>
         <v>42368.736851186717</v>
       </c>
@@ -2283,15 +2316,15 @@
       <c r="E22" s="22">
         <v>58904.8034364337</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="25">
         <f t="shared" ref="F22:F23" si="1">C22*0.8333</f>
         <v>235116.86784545748</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="26">
         <f t="shared" si="0"/>
         <v>209424.06738033245</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="27">
         <f t="shared" si="0"/>
         <v>49085.372703580208</v>
       </c>
@@ -2320,15 +2353,15 @@
       <c r="E23" s="22">
         <v>97049.563561422125</v>
       </c>
-      <c r="F23" s="31">
+      <c r="F23" s="28">
         <f t="shared" si="1"/>
         <v>326550.6030865967</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="29">
         <f t="shared" si="0"/>
         <v>308105.19913939532</v>
       </c>
-      <c r="H23" s="33">
+      <c r="H23" s="30">
         <f t="shared" si="0"/>
         <v>80871.401315733063</v>
       </c>

</xml_diff>

<commit_message>
Allow some heat pumps with no retrofit
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_RSD_Retrofit-Ctrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777D15F5-3C83-4F89-8334-08377A8ED51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8270B94B-77A0-415B-A38D-6EC4A08D9ADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$I$12</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>Deep Retrofit Required for Heat Pump</t>
+  </si>
+  <si>
+    <t>Share of 2030 retrofits</t>
   </si>
 </sst>
 </file>
@@ -695,7 +698,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -784,6 +787,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1941,12 +1947,12 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="47" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="2" customWidth="1"/>
@@ -1958,36 +1964,42 @@
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K4" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K5" s="38">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -2007,26 +2019,29 @@
         <v>2018</v>
       </c>
       <c r="G7" s="5">
+        <v>2030</v>
+      </c>
+      <c r="H7" s="5">
         <v>2070</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>"UC_RSD_DeepRetrofitCap-"&amp;J8</f>
+        <f>"UC_RSD_DeepRetrofitCap-"&amp;K8</f>
         <v>UC_RSD_DeepRetrofitCap-Apt</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;J8</f>
+        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;K8</f>
         <v>Maximum number of deep retrofitted dwellings in RSD Apt</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>"R-RTFT-"&amp;J8&amp;"_Deep"</f>
+        <f>"R-RTFT-"&amp;K8&amp;"_Deep"</f>
         <v>R-RTFT-Apt_Deep</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2040,27 +2055,31 @@
         <v>0</v>
       </c>
       <c r="G8" s="14">
+        <f>H8*$K$5</f>
+        <v>34.572524062475885</v>
+      </c>
+      <c r="H8" s="14">
         <f>(H23*G$15)/1000</f>
         <v>76.827831249946414</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str">
-        <f>"UC_RSD_ShallowRetrofitCap-"&amp;J9</f>
+        <f>"UC_RSD_ShallowRetrofitCap-"&amp;K9</f>
         <v>UC_RSD_ShallowRetrofitCap-Apt</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;J9</f>
+        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;K9</f>
         <v>Maximum number of deep retrofitted dwellings in RSD Apt</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f>"R-RTFT-"&amp;J9&amp;"_Shallow"</f>
+        <f>"R-RTFT-"&amp;K9&amp;"_Shallow"</f>
         <v>R-RTFT-Apt_Shallow</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -2074,27 +2093,31 @@
         <v>0</v>
       </c>
       <c r="G9" s="14">
+        <f t="shared" ref="G9:G13" si="0">H9*$K$5</f>
+        <v>20.983996830780541</v>
+      </c>
+      <c r="H9" s="14">
         <f>(H22*G$15)/1000</f>
         <v>46.6311040684012</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>"UC_RSD_DeepRetrofitCap-"&amp;J10</f>
+        <f>"UC_RSD_DeepRetrofitCap-"&amp;K10</f>
         <v>UC_RSD_DeepRetrofitCap-Att</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;J10</f>
+        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;K10</f>
         <v>Maximum number of deep retrofitted dwellings in RSD Att</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f>"R-RTFT-"&amp;J10&amp;"_Deep"</f>
+        <f>"R-RTFT-"&amp;K10&amp;"_Deep"</f>
         <v>R-RTFT-Att_Deep</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -2108,27 +2131,31 @@
         <v>0</v>
       </c>
       <c r="G10" s="14">
+        <f t="shared" si="0"/>
+        <v>139.60038281952009</v>
+      </c>
+      <c r="H10" s="14">
         <f>(F23*G$15)/1000</f>
         <v>310.22307293226686</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>5</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
-        <f>"UC_RSD_ShallowRetrofitCap-"&amp;J11</f>
+        <f>"UC_RSD_ShallowRetrofitCap-"&amp;K11</f>
         <v>UC_RSD_ShallowRetrofitCap-Att</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;J11</f>
+        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;K11</f>
         <v>Maximum number of deep retrofitted dwellings in RSD Att</v>
       </c>
       <c r="C11" s="2" t="str">
-        <f>"R-RTFT-"&amp;J11&amp;"_Shallow"</f>
+        <f>"R-RTFT-"&amp;K11&amp;"_Shallow"</f>
         <v>R-RTFT-Att_Shallow</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -2142,27 +2169,31 @@
         <v>0</v>
       </c>
       <c r="G11" s="14">
+        <f t="shared" si="0"/>
+        <v>100.51246100393307</v>
+      </c>
+      <c r="H11" s="14">
         <f>(F22*G$15)/1000</f>
         <v>223.3610244531846</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>"UC_RSD_DeepRetrofitCap-"&amp;J12</f>
+        <f>"UC_RSD_DeepRetrofitCap-"&amp;K12</f>
         <v>UC_RSD_DeepRetrofitCap-Det</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;J12</f>
+        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;K12</f>
         <v>Maximum number of deep retrofitted dwellings in RSD Det</v>
       </c>
       <c r="C12" s="31" t="str">
-        <f>"R-RTFT-"&amp;J12&amp;"_Deep"</f>
+        <f>"R-RTFT-"&amp;K12&amp;"_Deep"</f>
         <v>R-RTFT-Det_Deep</v>
       </c>
       <c r="D12" s="31" t="s">
@@ -2176,28 +2207,32 @@
         <v>0</v>
       </c>
       <c r="G12" s="14">
+        <f t="shared" si="0"/>
+        <v>131.7149726320915</v>
+      </c>
+      <c r="H12" s="14">
         <f>(G23*G$15)/1000</f>
         <v>292.69993918242557</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>5</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="31"/>
+      <c r="K12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
-        <f>"UC_RSD_ShallowRetrofitCap-"&amp;J13</f>
+        <f>"UC_RSD_ShallowRetrofitCap-"&amp;K13</f>
         <v>UC_RSD_ShallowRetrofitCap-Det</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;J13</f>
+        <f>"Maximum number of deep retrofitted dwellings in RSD "&amp;K13</f>
         <v>Maximum number of deep retrofitted dwellings in RSD Det</v>
       </c>
       <c r="C13" s="33" t="str">
-        <f>"R-RTFT-"&amp;J13&amp;"_Shallow"</f>
+        <f>"R-RTFT-"&amp;K13&amp;"_Shallow"</f>
         <v>R-RTFT-Det_Shallow</v>
       </c>
       <c r="D13" s="33" t="s">
@@ -2211,19 +2246,23 @@
         <v>0</v>
       </c>
       <c r="G13" s="34">
+        <f t="shared" si="0"/>
+        <v>89.528788805092105</v>
+      </c>
+      <c r="H13" s="34">
         <f>(G22*G$15)/1000</f>
         <v>198.9528640113158</v>
       </c>
-      <c r="H13" s="33">
+      <c r="I13" s="33">
         <v>5</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="31"/>
+      <c r="K13" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>76</v>
       </c>
@@ -2233,6 +2272,12 @@
       <c r="G15" s="20">
         <v>0.95</v>
       </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2308,11 +2353,11 @@
         <v>76933.418177245752</v>
       </c>
       <c r="G21" s="26">
-        <f t="shared" ref="G21:H23" si="0">D21*0.8333</f>
+        <f t="shared" ref="G21:H23" si="1">D21*0.8333</f>
         <v>86138.026655972135</v>
       </c>
       <c r="H21" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42368.736851186717</v>
       </c>
       <c r="L21" s="2" t="s">
@@ -2339,15 +2384,15 @@
         <v>58904.8034364337</v>
       </c>
       <c r="F22" s="25">
-        <f t="shared" ref="F22:F23" si="1">C22*0.8333</f>
+        <f t="shared" ref="F22:F23" si="2">C22*0.8333</f>
         <v>235116.86784545748</v>
       </c>
       <c r="G22" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>209424.06738033245</v>
       </c>
       <c r="H22" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49085.372703580208</v>
       </c>
       <c r="K22" s="3"/>
@@ -2376,15 +2421,15 @@
         <v>97049.563561422125</v>
       </c>
       <c r="F23" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>326550.6030865967</v>
       </c>
       <c r="G23" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>308105.19913939532</v>
       </c>
       <c r="H23" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80871.401315733063</v>
       </c>
     </row>
@@ -2403,6 +2448,18 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C26" s="2">
+        <f>C21/SUM(C22:C23)</f>
+        <v>0.1369732486903314</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" ref="D26:E26" si="3">D21/SUM(D22:D23)</f>
+        <v>0.16644088021385089</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.32602176509006114</v>
+      </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Gas Heat pumps to require retrofit but not Hybrids
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_RSD_Retrofit-Ctrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8270B94B-77A0-415B-A38D-6EC4A08D9ADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54898853-1A2A-4086-A826-14EFA409640C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -1947,7 +1947,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="K5" s="38">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="G8" s="14">
         <f>H8*$K$5</f>
-        <v>34.572524062475885</v>
+        <v>38.413915624973207</v>
       </c>
       <c r="H8" s="14">
         <f>(H23*G$15)/1000</f>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="G9" s="14">
         <f t="shared" ref="G9:G13" si="0">H9*$K$5</f>
-        <v>20.983996830780541</v>
+        <v>23.3155520342006</v>
       </c>
       <c r="H9" s="14">
         <f>(H22*G$15)/1000</f>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="G10" s="14">
         <f t="shared" si="0"/>
-        <v>139.60038281952009</v>
+        <v>155.11153646613343</v>
       </c>
       <c r="H10" s="14">
         <f>(F23*G$15)/1000</f>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="G11" s="14">
         <f t="shared" si="0"/>
-        <v>100.51246100393307</v>
+        <v>111.6805122265923</v>
       </c>
       <c r="H11" s="14">
         <f>(F22*G$15)/1000</f>
@@ -2208,7 +2208,7 @@
       </c>
       <c r="G12" s="14">
         <f t="shared" si="0"/>
-        <v>131.7149726320915</v>
+        <v>146.34996959121278</v>
       </c>
       <c r="H12" s="14">
         <f>(G23*G$15)/1000</f>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="G13" s="34">
         <f t="shared" si="0"/>
-        <v>89.528788805092105</v>
+        <v>99.476432005657898</v>
       </c>
       <c r="H13" s="34">
         <f>(G22*G$15)/1000</f>

</xml_diff>